<commit_message>
Add column to geoparsing summary for N cells
</commit_message>
<xml_diff>
--- a/outputs/geoparsing_cleaning_summary.xlsx
+++ b/outputs/geoparsing_cleaning_summary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Stage</t>
   </si>
@@ -36,15 +36,9 @@
     <t>Entity matching</t>
   </si>
   <si>
-    <t>All empirical studies with geoparsing matches</t>
-  </si>
-  <si>
     <t>Incorrect word to place match</t>
   </si>
   <si>
-    <t>Build a table of unique word x place matches and manually check the top 5% of most frequently occurring matches (which comprise 68\% of all matches) (see Supplementary Data file "geoparsing\_wordPlaceMatches95quantile\_cleaned.csv")</t>
-  </si>
-  <si>
     <t>Acronym falsely attributed to a geographical entity</t>
   </si>
   <si>
@@ -82,6 +76,18 @@
   </si>
   <si>
     <t>Remove grid cells that are attributed to a country that does not have a coastline bordering a match with a marine geographical entity match</t>
+  </si>
+  <si>
+    <t>N grid cells</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>All empirical articles with geoparsing matches</t>
+  </si>
+  <si>
+    <t>A table of unique word x place matches was used to manually check and correct the top 5% of most frequently occurring matches (which comprise 68\% of all matches) (see Supplementary Data file "geoparsing\_wordPlaceMatches95quantile\_cleaned.csv")</t>
   </si>
 </sst>
 </file>
@@ -117,13 +123,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -417,9 +426,10 @@
     <col min="2" max="2" width="22.08984375" customWidth="1"/>
     <col min="3" max="3" width="58.7265625" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,86 +442,91 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D9" s="1"/>
     </row>

</xml_diff>

<commit_message>
create summary of geoparsing steps
</commit_message>
<xml_diff>
--- a/outputs/geoparsing_cleaning_summary.xlsx
+++ b/outputs/geoparsing_cleaning_summary.xlsx
@@ -21,30 +21,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
-    <t>Stage</t>
-  </si>
-  <si>
     <t>Error type</t>
   </si>
   <si>
-    <t>Filter</t>
-  </si>
-  <si>
     <t>N articles</t>
   </si>
   <si>
-    <t>Entity matching</t>
-  </si>
-  <si>
     <t>Incorrect word to place match</t>
   </si>
   <si>
     <t>Acronym falsely attributed to a geographical entity</t>
   </si>
   <si>
-    <t>Remove acronym matches where the word matched is all capitalized letters, except UK and US</t>
-  </si>
-  <si>
     <t>Copyright/publisher location appearing in article abstract text and returning a geographical entity match</t>
   </si>
   <si>
@@ -63,31 +51,43 @@
     <t>Remove matches that contain a number or contains a scientific species name or ecosystem/marine system type (e.g. "estuary").</t>
   </si>
   <si>
-    <t>Matching entities to grid cells</t>
-  </si>
-  <si>
     <t>Geographical entity is matched correctly, but unlikely to be representative of an empirical study location</t>
   </si>
   <si>
     <t>Retain only matches to terrestrial grid cells within 200 km of the coastline.</t>
   </si>
   <si>
-    <t>Shapefile gridding attributing matches to erroneous countries</t>
-  </si>
-  <si>
-    <t>Remove grid cells that are attributed to a country that does not have a coastline bordering a match with a marine geographical entity match</t>
-  </si>
-  <si>
     <t>N grid cells</t>
   </si>
   <si>
     <t>NA</t>
   </si>
   <si>
-    <t>All empirical articles with geoparsing matches</t>
-  </si>
-  <si>
     <t>A table of unique word x place matches was used to manually check and correct the top 5% of most frequently occurring matches (which comprise 68\% of all matches) (see Supplementary Data file "geoparsing\_wordPlaceMatches95quantile\_cleaned.csv")</t>
+  </si>
+  <si>
+    <t>Data cleaning step</t>
+  </si>
+  <si>
+    <t>Start with all empirical articles with geoparsing matches</t>
+  </si>
+  <si>
+    <t>Remove acronym matches where the word matched is all capitalized letters and less than 3 characters long, except UK, US, and USA</t>
+  </si>
+  <si>
+    <t>Geographical entities mentioned that are not representative of where the study was conducted (e.g. locations being listed in abstract text as part of an introductory sentence providing examples of other case studies)</t>
+  </si>
+  <si>
+    <t>When there is a geographical entity in the title or keywords, retain only that entity match and discard others in abstract text</t>
+  </si>
+  <si>
+    <t>Since our analysis is focused on national research effort, there is no need to retain matches in the high seas that cannot be attributed to a country</t>
+  </si>
+  <si>
+    <t>Remove grid cell matches in the high seas</t>
+  </si>
+  <si>
+    <t>Counts after cleaning step is applied</t>
   </si>
 </sst>
 </file>
@@ -111,7 +111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -119,21 +119,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,127 +434,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.90625" customWidth="1"/>
-    <col min="2" max="2" width="22.08984375" customWidth="1"/>
-    <col min="3" max="3" width="58.7265625" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="58.7265625" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1107767</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6530</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1094923</v>
+      </c>
+      <c r="D4" s="3">
+        <v>6436</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1080904</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2">
+        <v>398605</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5608</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2">
+        <v>385197</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>379630</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5503</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2">
+        <v>342213</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="C10" s="2">
+        <v>262910</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1"/>
+      <c r="C11" s="7">
+        <v>261957</v>
+      </c>
+      <c r="D11" s="8">
+        <v>5194</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A9"/>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>